<commit_message>
[master]  * Modification du mapping
</commit_message>
<xml_diff>
--- a/master/DOCS/mapping.xlsx
+++ b/master/DOCS/mapping.xlsx
@@ -59,172 +59,172 @@
     <t xml:space="preserve">PP0</t>
   </si>
   <si>
+    <t xml:space="preserve">PC4 UART7 Rx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB1  UART1 TX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC5 UART7 Tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">see JP4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">see JP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB4 SSI2Clk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PQ0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD3 SSI2Clk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA6 I2C1SCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB2 I2C0SCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA7 I2C1SDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PN4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB3 I2C0SDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(PG1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PF3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PB3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PK5</t>
+  </si>
+  <si>
     <t xml:space="preserve">PC4</t>
   </si>
   <si>
-    <t xml:space="preserve">PB1  UART1 TX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PP1</t>
+    <t xml:space="preserve">PM0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PG0</t>
   </si>
   <si>
     <t xml:space="preserve">PC5</t>
   </si>
   <si>
-    <t xml:space="preserve">see JP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC6 UART TX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">see JP5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE5 UART RX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB4 SSI2Clk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PQ0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD3 SSI2Clk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA6 I2C1SCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PN5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB2 I2C0SCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA7 I2C1SDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PN4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB3 I2C0SDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PK0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PK1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PK2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PD7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PK3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PA4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(PG1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PF3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PK4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PB3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PK5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PG0</t>
-  </si>
-  <si>
     <t xml:space="preserve">PM1</t>
   </si>
   <si>
     <t xml:space="preserve">PL4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC6</t>
   </si>
   <si>
     <t xml:space="preserve">PM2</t>
@@ -870,7 +870,7 @@
   <dimension ref="B1:D49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -966,106 +966,106 @@
         <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,114 +1073,114 @@
         <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>62</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="5" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>63</v>
@@ -1191,18 +1191,18 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="5" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="5" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>68</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>70</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>75</v>
@@ -1268,13 +1268,13 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,7 +1345,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>99</v>
@@ -1557,10 +1557,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>124</v>

</xml_diff>